<commit_message>
Fix: Match CSM in ifrs17a
</commit_message>
<xml_diff>
--- a/lifelib/libraries/ifrs17a/tests/expected/template.xlsx
+++ b/lifelib/libraries/ifrs17a/tests/expected/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e058ec69bd94c7d/pyproj/lifelib/lifelib/libraries/ifrs17a/tests/expected/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_496D53BF455F122EEB75ECF65BB7663F935B83D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{431CB9C6-4201-4C42-8556-C80878757F54}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_496D53BF455F122EEB75ECF65BB7663F935B83D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF7339A9-E6DF-4716-AADF-DA37EFFBB25B}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="3720" windowWidth="31440" windowHeight="17040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="2410" windowWidth="16670" windowHeight="17040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BE" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +149,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,16 +189,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1276,37 +1333,37 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2">
-        <v>-5.0896213913131163</v>
+        <v>-18.986560525490869</v>
       </c>
       <c r="D2">
         <v>-8.1282965710591668</v>
@@ -1316,8 +1373,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -1331,8 +1388,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C4">
@@ -1346,12 +1403,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>24.55456452110511</v>
+        <v>39.887800253531921</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1361,14 +1418,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>185.66499029753831</v>
+        <v>228.73571029973269</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1378,8 +1435,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7">
@@ -1393,12 +1450,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8">
-        <v>0.35734074449602637</v>
+        <v>0.37885997179469488</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1408,8 +1465,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9">
@@ -1423,10 +1480,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10">
@@ -1440,8 +1497,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C11">
@@ -1455,8 +1512,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12">

</xml_diff>